<commit_message>
Putting Number of candidates in Config File
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPath\POC\POC-Dispatcher_Performer_Model\POC-Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BEBC6E-CA9B-4068-8A4E-A911A393B8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2643C1D-89C2-412A-9F9E-81887F995388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>D:\UIPath\POC\POC-Dispatcher_Performer_Model\POC-Performer\Data\Output\Candidate List.xlsx</t>
+  </si>
+  <si>
+    <t>NumberOfCandidates</t>
   </si>
 </sst>
 </file>
@@ -588,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -730,7 +733,14 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+    </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added Linkedin Logout Functionality
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPath\POC\POC-Dispatcher_Performer_Model\POC-Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2643C1D-89C2-412A-9F9E-81887F995388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63C7607-2491-4942-9974-24C58F98F439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>NumberOfCandidates</t>
+  </si>
+  <si>
+    <t>LinkedinHomePage</t>
   </si>
 </sst>
 </file>
@@ -592,7 +595,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -742,7 +745,14 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>